<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758703540744_admin@admin.com.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758703540744_admin@admin.com.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758703540744_admin@admin.com.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAAB535-302E-48CF-88AC-CA475A1E66E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF2C70-7C3C-4A12-A0FD-BB29B60D20ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="580" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Surgery" sheetId="1" r:id="rId1"/>
@@ -380,10 +380,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -412,7 +419,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,16 +761,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D109"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="10.25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -783,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -794,7 +801,7 @@
         <v>45915</v>
       </c>
       <c r="D2" s="2">
-        <v>0.46875</v>
+        <v>0.46059027777777778</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -803,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -814,7 +821,7 @@
         <v>45915</v>
       </c>
       <c r="D3" s="2">
-        <v>0.46875</v>
+        <v>0.46059027777777778</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -823,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -834,7 +841,7 @@
         <v>45915</v>
       </c>
       <c r="D4" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -843,7 +850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -854,7 +861,7 @@
         <v>45915</v>
       </c>
       <c r="D5" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -863,7 +870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -874,7 +881,7 @@
         <v>45915</v>
       </c>
       <c r="D6" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -883,7 +890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -894,7 +901,7 @@
         <v>45915</v>
       </c>
       <c r="D7" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -903,7 +910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -914,7 +921,7 @@
         <v>45915</v>
       </c>
       <c r="D8" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -923,7 +930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -934,7 +941,7 @@
         <v>45915</v>
       </c>
       <c r="D9" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -943,7 +950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -954,7 +961,7 @@
         <v>45915</v>
       </c>
       <c r="D10" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -963,7 +970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -974,7 +981,7 @@
         <v>45915</v>
       </c>
       <c r="D11" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -983,7 +990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -994,7 +1001,7 @@
         <v>45915</v>
       </c>
       <c r="D12" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1003,7 +1010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1014,7 +1021,7 @@
         <v>45915</v>
       </c>
       <c r="D13" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1023,7 +1030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1034,7 +1041,7 @@
         <v>45915</v>
       </c>
       <c r="D14" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1043,7 +1050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>45915</v>
       </c>
       <c r="D15" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1063,7 +1070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1074,7 +1081,7 @@
         <v>45915</v>
       </c>
       <c r="D16" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1083,7 +1090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1094,7 +1101,7 @@
         <v>45915</v>
       </c>
       <c r="D17" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -1103,7 +1110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1114,7 +1121,7 @@
         <v>45915</v>
       </c>
       <c r="D18" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1123,7 +1130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1134,7 +1141,7 @@
         <v>45915</v>
       </c>
       <c r="D19" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1143,7 +1150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1154,7 +1161,7 @@
         <v>45915</v>
       </c>
       <c r="D20" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1163,7 +1170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1174,7 +1181,7 @@
         <v>45915</v>
       </c>
       <c r="D21" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1183,7 +1190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>45915</v>
       </c>
       <c r="D22" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1203,7 +1210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1214,7 +1221,7 @@
         <v>45915</v>
       </c>
       <c r="D23" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1223,7 +1230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1234,7 +1241,7 @@
         <v>45915</v>
       </c>
       <c r="D24" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1243,7 +1250,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1254,7 +1261,7 @@
         <v>45915</v>
       </c>
       <c r="D25" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1263,7 +1270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1274,7 +1281,7 @@
         <v>45915</v>
       </c>
       <c r="D26" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1283,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1294,7 +1301,7 @@
         <v>45915</v>
       </c>
       <c r="D27" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1303,7 +1310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1314,7 +1321,7 @@
         <v>45915</v>
       </c>
       <c r="D28" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -1323,7 +1330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1334,7 +1341,7 @@
         <v>45915</v>
       </c>
       <c r="D29" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1343,7 +1350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1354,7 +1361,7 @@
         <v>45915</v>
       </c>
       <c r="D30" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -1363,7 +1370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1374,7 +1381,7 @@
         <v>45915</v>
       </c>
       <c r="D31" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -1383,7 +1390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1394,7 +1401,7 @@
         <v>45915</v>
       </c>
       <c r="D32" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
@@ -1403,7 +1410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1414,7 +1421,7 @@
         <v>45915</v>
       </c>
       <c r="D33" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1423,7 +1430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1434,7 +1441,7 @@
         <v>45915</v>
       </c>
       <c r="D34" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E34" t="s">
         <v>41</v>
@@ -1443,7 +1450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1454,7 +1461,7 @@
         <v>45915</v>
       </c>
       <c r="D35" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E35" t="s">
         <v>41</v>
@@ -1463,7 +1470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1474,7 +1481,7 @@
         <v>45915</v>
       </c>
       <c r="D36" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E36" t="s">
         <v>41</v>
@@ -1483,7 +1490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1494,7 +1501,7 @@
         <v>45915</v>
       </c>
       <c r="D37" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E37" t="s">
         <v>41</v>
@@ -1503,7 +1510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1514,7 +1521,7 @@
         <v>45915</v>
       </c>
       <c r="D38" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E38" t="s">
         <v>41</v>
@@ -1523,7 +1530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1534,7 +1541,7 @@
         <v>45915</v>
       </c>
       <c r="D39" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E39" t="s">
         <v>41</v>
@@ -1543,7 +1550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1554,7 +1561,7 @@
         <v>45915</v>
       </c>
       <c r="D40" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E40" t="s">
         <v>41</v>
@@ -1563,7 +1570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1574,7 +1581,7 @@
         <v>45915</v>
       </c>
       <c r="D41" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E41" t="s">
         <v>41</v>
@@ -1583,7 +1590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1594,7 +1601,7 @@
         <v>45915</v>
       </c>
       <c r="D42" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E42" t="s">
         <v>41</v>
@@ -1603,7 +1610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -1614,7 +1621,7 @@
         <v>45915</v>
       </c>
       <c r="D43" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E43" t="s">
         <v>41</v>
@@ -1623,7 +1630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1634,7 +1641,7 @@
         <v>45915</v>
       </c>
       <c r="D44" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
@@ -1643,7 +1650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1654,7 +1661,7 @@
         <v>45915</v>
       </c>
       <c r="D45" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E45" t="s">
         <v>41</v>
@@ -1663,7 +1670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1674,7 +1681,7 @@
         <v>45915</v>
       </c>
       <c r="D46" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -1683,7 +1690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1694,7 +1701,7 @@
         <v>45915</v>
       </c>
       <c r="D47" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1703,7 +1710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1714,7 +1721,7 @@
         <v>45915</v>
       </c>
       <c r="D48" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -1723,7 +1730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1734,7 +1741,7 @@
         <v>45915</v>
       </c>
       <c r="D49" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E49" t="s">
         <v>41</v>
@@ -1743,7 +1750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1754,7 +1761,7 @@
         <v>45915</v>
       </c>
       <c r="D50" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E50" t="s">
         <v>41</v>
@@ -1763,7 +1770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1774,7 +1781,7 @@
         <v>45915</v>
       </c>
       <c r="D51" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
@@ -1783,7 +1790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1794,7 +1801,7 @@
         <v>45915</v>
       </c>
       <c r="D52" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E52" t="s">
         <v>41</v>
@@ -1803,7 +1810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1814,7 +1821,7 @@
         <v>45915</v>
       </c>
       <c r="D53" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E53" t="s">
         <v>41</v>
@@ -1823,7 +1830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -1834,7 +1841,7 @@
         <v>45915</v>
       </c>
       <c r="D54" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
@@ -1843,7 +1850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1854,7 +1861,7 @@
         <v>45915</v>
       </c>
       <c r="D55" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
@@ -1863,7 +1870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1874,7 +1881,7 @@
         <v>45915</v>
       </c>
       <c r="D56" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
@@ -1883,7 +1890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1894,7 +1901,7 @@
         <v>45915</v>
       </c>
       <c r="D57" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E57" t="s">
         <v>8</v>
@@ -1903,7 +1910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1914,7 +1921,7 @@
         <v>45915</v>
       </c>
       <c r="D58" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
@@ -1923,7 +1930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -1934,7 +1941,7 @@
         <v>45915</v>
       </c>
       <c r="D59" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E59" t="s">
         <v>8</v>
@@ -1943,7 +1950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1954,7 +1961,7 @@
         <v>45915</v>
       </c>
       <c r="D60" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E60" t="s">
         <v>8</v>
@@ -1963,7 +1970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1974,7 +1981,7 @@
         <v>45915</v>
       </c>
       <c r="D61" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
@@ -1983,7 +1990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -1994,7 +2001,7 @@
         <v>45915</v>
       </c>
       <c r="D62" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E62" t="s">
         <v>8</v>
@@ -2003,7 +2010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -2014,7 +2021,7 @@
         <v>45915</v>
       </c>
       <c r="D63" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E63" t="s">
         <v>8</v>
@@ -2023,7 +2030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -2034,7 +2041,7 @@
         <v>45915</v>
       </c>
       <c r="D64" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E64" t="s">
         <v>8</v>
@@ -2043,7 +2050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -2054,7 +2061,7 @@
         <v>45915</v>
       </c>
       <c r="D65" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E65" t="s">
         <v>8</v>
@@ -2063,7 +2070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -2074,7 +2081,7 @@
         <v>45915</v>
       </c>
       <c r="D66" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E66" t="s">
         <v>8</v>
@@ -2083,7 +2090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -2094,7 +2101,7 @@
         <v>45915</v>
       </c>
       <c r="D67" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E67" t="s">
         <v>8</v>
@@ -2103,7 +2110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -2114,7 +2121,7 @@
         <v>45915</v>
       </c>
       <c r="D68" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
@@ -2123,7 +2130,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2134,7 +2141,7 @@
         <v>45915</v>
       </c>
       <c r="D69" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E69" t="s">
         <v>8</v>
@@ -2143,7 +2150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -2154,7 +2161,7 @@
         <v>45915</v>
       </c>
       <c r="D70" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -2163,7 +2170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -2174,7 +2181,7 @@
         <v>45915</v>
       </c>
       <c r="D71" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E71" t="s">
         <v>8</v>
@@ -2183,7 +2190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2194,7 +2201,7 @@
         <v>45915</v>
       </c>
       <c r="D72" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E72" t="s">
         <v>41</v>
@@ -2203,7 +2210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -2214,7 +2221,7 @@
         <v>45915</v>
       </c>
       <c r="D73" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -2223,7 +2230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -2234,7 +2241,7 @@
         <v>45915</v>
       </c>
       <c r="D74" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E74" t="s">
         <v>41</v>
@@ -2243,7 +2250,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -2254,7 +2261,7 @@
         <v>45915</v>
       </c>
       <c r="D75" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E75" t="s">
         <v>8</v>
@@ -2263,7 +2270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -2274,7 +2281,7 @@
         <v>45915</v>
       </c>
       <c r="D76" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E76" t="s">
         <v>41</v>
@@ -2283,7 +2290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -2294,7 +2301,7 @@
         <v>45915</v>
       </c>
       <c r="D77" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
@@ -2303,7 +2310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -2314,7 +2321,7 @@
         <v>45915</v>
       </c>
       <c r="D78" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E78" t="s">
         <v>8</v>
@@ -2323,7 +2330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -2334,7 +2341,7 @@
         <v>45915</v>
       </c>
       <c r="D79" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E79" t="s">
         <v>8</v>
@@ -2343,7 +2350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2354,7 +2361,7 @@
         <v>45915</v>
       </c>
       <c r="D80" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2363,7 +2370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -2374,7 +2381,7 @@
         <v>45915</v>
       </c>
       <c r="D81" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E81" t="s">
         <v>8</v>
@@ -2383,7 +2390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2394,7 +2401,7 @@
         <v>45915</v>
       </c>
       <c r="D82" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E82" t="s">
         <v>41</v>
@@ -2403,7 +2410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -2414,7 +2421,7 @@
         <v>45915</v>
       </c>
       <c r="D83" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
@@ -2423,7 +2430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -2434,7 +2441,7 @@
         <v>45915</v>
       </c>
       <c r="D84" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2443,7 +2450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -2454,7 +2461,7 @@
         <v>45915</v>
       </c>
       <c r="D85" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
@@ -2463,7 +2470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -2474,7 +2481,7 @@
         <v>45915</v>
       </c>
       <c r="D86" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E86" t="s">
         <v>8</v>
@@ -2483,7 +2490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -2494,7 +2501,7 @@
         <v>45915</v>
       </c>
       <c r="D87" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E87" t="s">
         <v>8</v>
@@ -2503,7 +2510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -2514,7 +2521,7 @@
         <v>45915</v>
       </c>
       <c r="D88" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E88" t="s">
         <v>8</v>
@@ -2523,7 +2530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -2534,7 +2541,7 @@
         <v>45915</v>
       </c>
       <c r="D89" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E89" t="s">
         <v>8</v>
@@ -2543,7 +2550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -2554,7 +2561,7 @@
         <v>45915</v>
       </c>
       <c r="D90" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E90" t="s">
         <v>8</v>
@@ -2563,7 +2570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -2574,7 +2581,7 @@
         <v>45915</v>
       </c>
       <c r="D91" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
@@ -2583,7 +2590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -2594,7 +2601,7 @@
         <v>45915</v>
       </c>
       <c r="D92" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E92" t="s">
         <v>8</v>
@@ -2603,7 +2610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -2614,7 +2621,7 @@
         <v>45915</v>
       </c>
       <c r="D93" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E93" t="s">
         <v>8</v>
@@ -2623,7 +2630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -2634,7 +2641,7 @@
         <v>45915</v>
       </c>
       <c r="D94" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E94" t="s">
         <v>8</v>
@@ -2643,7 +2650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -2654,7 +2661,7 @@
         <v>45915</v>
       </c>
       <c r="D95" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E95" t="s">
         <v>8</v>
@@ -2663,7 +2670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -2674,7 +2681,7 @@
         <v>45915</v>
       </c>
       <c r="D96" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E96" t="s">
         <v>8</v>
@@ -2683,7 +2690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>105</v>
       </c>
@@ -2694,7 +2701,7 @@
         <v>45915</v>
       </c>
       <c r="D97" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E97" t="s">
         <v>8</v>
@@ -2703,7 +2710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>106</v>
       </c>
@@ -2714,7 +2721,7 @@
         <v>45915</v>
       </c>
       <c r="D98" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E98" t="s">
         <v>8</v>
@@ -2723,7 +2730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>107</v>
       </c>
@@ -2734,7 +2741,7 @@
         <v>45915</v>
       </c>
       <c r="D99" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E99" t="s">
         <v>8</v>
@@ -2743,7 +2750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>108</v>
       </c>
@@ -2754,7 +2761,7 @@
         <v>45915</v>
       </c>
       <c r="D100" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E100" t="s">
         <v>8</v>
@@ -2763,7 +2770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>109</v>
       </c>
@@ -2774,7 +2781,7 @@
         <v>45915</v>
       </c>
       <c r="D101" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E101" t="s">
         <v>41</v>
@@ -2783,7 +2790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>110</v>
       </c>
@@ -2794,7 +2801,7 @@
         <v>45915</v>
       </c>
       <c r="D102" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E102" t="s">
         <v>41</v>
@@ -2803,7 +2810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>111</v>
       </c>
@@ -2814,7 +2821,7 @@
         <v>45915</v>
       </c>
       <c r="D103" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E103" t="s">
         <v>8</v>
@@ -2823,7 +2830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>112</v>
       </c>
@@ -2834,7 +2841,7 @@
         <v>45915</v>
       </c>
       <c r="D104" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E104" t="s">
         <v>8</v>
@@ -2843,7 +2850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>113</v>
       </c>
@@ -2854,7 +2861,7 @@
         <v>45915</v>
       </c>
       <c r="D105" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E105" t="s">
         <v>8</v>
@@ -2863,7 +2870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -2874,7 +2881,7 @@
         <v>45915</v>
       </c>
       <c r="D106" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E106" t="s">
         <v>8</v>
@@ -2883,7 +2890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>115</v>
       </c>
@@ -2894,7 +2901,7 @@
         <v>45915</v>
       </c>
       <c r="D107" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E107" t="s">
         <v>8</v>
@@ -2903,7 +2910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>116</v>
       </c>
@@ -2914,7 +2921,7 @@
         <v>45915</v>
       </c>
       <c r="D108" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E108" t="s">
         <v>8</v>
@@ -2923,7 +2930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>117</v>
       </c>
@@ -2934,7 +2941,7 @@
         <v>45915</v>
       </c>
       <c r="D109" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E109" t="s">
         <v>8</v>

</xml_diff>